<commit_message>
Changed mast to motors. Added tote pincher. Changed setPosition to setAngle
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21105" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Channel Assignments" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="50">
   <si>
     <t>Function</t>
   </si>
@@ -157,6 +158,15 @@
   </si>
   <si>
     <t>practiceRobot</t>
+  </si>
+  <si>
+    <t>mastLeft</t>
+  </si>
+  <si>
+    <t>mastRight</t>
+  </si>
+  <si>
+    <t>mastPot</t>
   </si>
 </sst>
 </file>
@@ -172,12 +182,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -268,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -294,6 +316,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -303,7 +328,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,11 +657,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -647,7 +681,7 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="2"/>
@@ -659,7 +693,7 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D4" s="2"/>
@@ -671,7 +705,7 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="2"/>
@@ -683,7 +717,7 @@
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="2"/>
@@ -695,7 +729,7 @@
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="2"/>
@@ -707,7 +741,7 @@
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="2"/>
@@ -719,7 +753,7 @@
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2"/>
@@ -731,7 +765,7 @@
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D10" s="2"/>
@@ -916,11 +950,11 @@
       <c r="D28" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
@@ -1003,7 +1037,7 @@
       <c r="B36" s="3">
         <v>4</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="11" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="2"/>
@@ -1093,9 +1127,13 @@
       <c r="B42" s="4">
         <v>10</v>
       </c>
-      <c r="C42" s="10"/>
+      <c r="C42" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
@@ -1104,9 +1142,13 @@
       <c r="B43" s="3">
         <v>11</v>
       </c>
-      <c r="C43" s="10"/>
+      <c r="C43" s="17" t="s">
+        <v>48</v>
+      </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
@@ -1197,11 +1239,11 @@
       <c r="E51" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
@@ -1221,7 +1263,7 @@
       <c r="B55" s="3">
         <v>0</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="2"/>
@@ -1233,7 +1275,7 @@
       <c r="B56" s="3">
         <v>1</v>
       </c>
-      <c r="C56" s="3"/>
+      <c r="C56" s="9"/>
       <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1243,7 +1285,7 @@
       <c r="B57" s="3">
         <v>2</v>
       </c>
-      <c r="C57" s="3"/>
+      <c r="C57" s="9"/>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1253,15 +1295,15 @@
       <c r="B58" s="3">
         <v>3</v>
       </c>
-      <c r="C58" s="3"/>
+      <c r="C58" s="9"/>
       <c r="D58" s="2"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="14"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
@@ -1281,7 +1323,7 @@
       <c r="B62" s="3">
         <v>0</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="9" t="s">
         <v>40</v>
       </c>
       <c r="D62" s="2"/>
@@ -1293,7 +1335,7 @@
       <c r="B63" s="3">
         <v>1</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="9" t="s">
         <v>41</v>
       </c>
       <c r="D63" s="2"/>
@@ -1305,7 +1347,7 @@
       <c r="B64" s="3">
         <v>2</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D64" s="2"/>
@@ -1317,7 +1359,9 @@
       <c r="B65" s="3">
         <v>3</v>
       </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1327,7 +1371,7 @@
       <c r="B66" s="5">
         <v>4</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="2"/>
@@ -1339,7 +1383,7 @@
       <c r="B67" s="5">
         <v>5</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D67" s="2"/>
@@ -1351,7 +1395,7 @@
       <c r="B68" s="5">
         <v>6</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D68" s="2"/>
@@ -1363,15 +1407,15 @@
       <c r="B69" s="5">
         <v>7</v>
       </c>
-      <c r="C69" s="2"/>
+      <c r="C69" s="10"/>
       <c r="D69" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="14"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
@@ -1391,7 +1435,7 @@
       <c r="B73" s="3">
         <v>0</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" s="9" t="s">
         <v>44</v>
       </c>
       <c r="D73" s="2"/>
@@ -1403,7 +1447,7 @@
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="18" t="s">
         <v>42</v>
       </c>
       <c r="D74" s="2"/>
@@ -1415,7 +1459,7 @@
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D75" s="2"/>
@@ -1427,7 +1471,7 @@
       <c r="B76" s="3">
         <v>3</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D76" s="2"/>
@@ -1439,7 +1483,7 @@
       <c r="B77" s="5">
         <v>4</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D77" s="2"/>
@@ -1451,7 +1495,7 @@
       <c r="B78" s="5">
         <v>5</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D78" s="2"/>
@@ -1463,7 +1507,7 @@
       <c r="B79" s="5">
         <v>6</v>
       </c>
-      <c r="C79" s="2"/>
+      <c r="C79" s="10"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,7 +1517,7 @@
       <c r="B80" s="5">
         <v>7</v>
       </c>
-      <c r="C80" s="2"/>
+      <c r="C80" s="10"/>
       <c r="D80" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Jaguars to VictorSP per Matt
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="21105" windowHeight="8685"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="21108" windowHeight="8688"/>
   </bookViews>
   <sheets>
     <sheet name="Channel Assignments" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
   <si>
     <t>Function</t>
   </si>
@@ -116,9 +115,6 @@
   </si>
   <si>
     <t>buzzer</t>
-  </si>
-  <si>
-    <t>Jaguar</t>
   </si>
   <si>
     <t>driveTrainEncoderL_A</t>
@@ -172,8 +168,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -290,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -319,15 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -340,6 +333,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +432,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -464,7 +466,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -640,30 +641,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="17"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -674,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,11 +683,11 @@
         <v>0</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -694,11 +695,11 @@
         <v>1</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -710,7 +711,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -722,31 +723,31 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>36</v>
+      <c r="C7" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>37</v>
+      <c r="C8" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -758,7 +759,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -766,11 +767,11 @@
         <v>7</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -779,7 +780,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -789,7 +790,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -799,7 +800,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -809,7 +810,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
@@ -819,7 +820,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
@@ -829,7 +830,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -839,7 +840,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -849,7 +850,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
@@ -859,7 +860,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -869,7 +870,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
@@ -879,7 +880,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -889,7 +890,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -899,7 +900,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
@@ -909,7 +910,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
@@ -919,7 +920,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -929,7 +930,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
@@ -939,7 +940,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
@@ -949,14 +950,14 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+    <row r="30" spans="1:5">
+      <c r="B30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:5">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
@@ -970,7 +971,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -985,7 +986,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -1000,7 +1001,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1038,14 +1039,14 @@
         <v>4</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1053,14 +1054,14 @@
         <v>5</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
         <v>6</v>
       </c>
@@ -1075,7 +1076,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1101,11 +1102,11 @@
         <v>17</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1116,41 +1117,41 @@
         <v>16</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="4">
         <v>10</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>47</v>
+      <c r="C42" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="3">
         <v>11</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>48</v>
+      <c r="C43" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="8" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1162,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="8" t="s">
         <v>7</v>
       </c>
@@ -1172,7 +1173,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="8" t="s">
         <v>7</v>
       </c>
@@ -1183,7 +1184,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="8" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1195,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="8" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1206,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49" s="8" t="s">
         <v>7</v>
       </c>
@@ -1216,7 +1217,7 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50" s="8" t="s">
         <v>7</v>
       </c>
@@ -1227,7 +1228,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="8" t="s">
         <v>7</v>
       </c>
@@ -1238,14 +1239,14 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
+    <row r="53" spans="1:5">
+      <c r="B53" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="14"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+    </row>
+    <row r="54" spans="1:5">
       <c r="B54" s="1" t="s">
         <v>1</v>
       </c>
@@ -1256,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
@@ -1268,7 +1269,7 @@
       </c>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
@@ -1278,7 +1279,7 @@
       <c r="C56" s="9"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
         <v>6</v>
       </c>
@@ -1288,7 +1289,7 @@
       <c r="C57" s="9"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
@@ -1298,14 +1299,14 @@
       <c r="C58" s="9"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="12" t="s">
+    <row r="60" spans="1:5">
+      <c r="B60" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="17"/>
+      <c r="D60" s="18"/>
+    </row>
+    <row r="61" spans="1:5">
       <c r="B61" s="6" t="s">
         <v>1</v>
       </c>
@@ -1316,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
         <v>6</v>
       </c>
@@ -1324,11 +1325,11 @@
         <v>0</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1336,11 +1337,11 @@
         <v>1</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
         <v>6</v>
       </c>
@@ -1352,19 +1353,19 @@
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B65" s="3">
         <v>3</v>
       </c>
-      <c r="C65" s="16" t="s">
-        <v>49</v>
+      <c r="C65" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>7</v>
       </c>
@@ -1376,7 +1377,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>7</v>
       </c>
@@ -1388,7 +1389,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>7</v>
       </c>
@@ -1400,7 +1401,7 @@
       </c>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>7</v>
       </c>
@@ -1410,14 +1411,14 @@
       <c r="C69" s="10"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="12" t="s">
+    <row r="71" spans="1:4">
+      <c r="B71" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="13"/>
-      <c r="D71" s="14"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="17"/>
+      <c r="D71" s="18"/>
+    </row>
+    <row r="72" spans="1:4">
       <c r="B72" s="6" t="s">
         <v>1</v>
       </c>
@@ -1428,45 +1429,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
       </c>
       <c r="C73" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="18" t="s">
-        <v>42</v>
+      <c r="C74" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="18" t="s">
-        <v>43</v>
+      <c r="C75" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B76" s="3">
         <v>3</v>
@@ -1476,9 +1477,9 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B77" s="5">
         <v>4</v>
@@ -1488,9 +1489,9 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B78" s="5">
         <v>5</v>
@@ -1500,9 +1501,9 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B79" s="5">
         <v>6</v>
@@ -1510,9 +1511,9 @@
       <c r="C79" s="10"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B80" s="5">
         <v>7</v>
@@ -1533,24 +1534,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Make everything DualSpeedControllers. Rearrange DIO to match 2014.
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -333,6 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -342,7 +343,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -658,11 +658,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -682,8 +682,8 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>33</v>
+      <c r="C3" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -694,8 +694,8 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>34</v>
+      <c r="C4" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -706,9 +706,7 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
@@ -718,9 +716,7 @@
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>31</v>
-      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
@@ -730,8 +726,8 @@
       <c r="B7" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>35</v>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -742,8 +738,8 @@
       <c r="B8" s="3">
         <v>5</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>36</v>
+      <c r="C8" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="D8" s="2"/>
     </row>
@@ -755,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2"/>
     </row>
@@ -766,8 +762,8 @@
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>45</v>
+      <c r="C10" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -778,6 +774,9 @@
       <c r="B11" s="3">
         <v>8</v>
       </c>
+      <c r="C11" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4">
@@ -787,7 +786,9 @@
       <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4">
@@ -797,7 +798,7 @@
       <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
@@ -827,7 +828,7 @@
       <c r="B16" s="5">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:5">
@@ -951,11 +952,11 @@
       <c r="D28" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="1" t="s">
@@ -1102,7 +1103,7 @@
         <v>17</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1117,7 +1118,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1240,11 +1241,11 @@
       <c r="E51" s="2"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="18"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="19"/>
     </row>
     <row r="54" spans="1:5">
       <c r="B54" s="1" t="s">
@@ -1300,11 +1301,11 @@
       <c r="D58" s="2"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="19"/>
     </row>
     <row r="61" spans="1:5">
       <c r="B61" s="6" t="s">
@@ -1412,11 +1413,11 @@
       <c r="D69" s="2"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="19"/>
     </row>
     <row r="72" spans="1:4">
       <c r="B72" s="6" t="s">

</xml_diff>

<commit_message>
Updates per Shane and Lauren
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -123,30 +123,12 @@
     <t>driveTrainEncoderL_B</t>
   </si>
   <si>
-    <t>pickupEncoderA</t>
-  </si>
-  <si>
-    <t>pickupEncoderB</t>
-  </si>
-  <si>
-    <t>pickupLiftLeft</t>
-  </si>
-  <si>
-    <t>pickupLiftRight</t>
-  </si>
-  <si>
     <t>wristPot</t>
   </si>
   <si>
     <t>armPot</t>
   </si>
   <si>
-    <t>mast(forward)</t>
-  </si>
-  <si>
-    <t>mast(reverse)</t>
-  </si>
-  <si>
     <t>shift</t>
   </si>
   <si>
@@ -163,13 +145,31 @@
   </si>
   <si>
     <t>mastPot</t>
+  </si>
+  <si>
+    <t>mastLock</t>
+  </si>
+  <si>
+    <t>totePincher</t>
+  </si>
+  <si>
+    <t>liftLeft</t>
+  </si>
+  <si>
+    <t>liftRight</t>
+  </si>
+  <si>
+    <t>liftEncoderA</t>
+  </si>
+  <si>
+    <t>liftEncoderB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,8 +177,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,19 +193,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,13 +321,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -342,6 +329,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -658,11 +648,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -683,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -695,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -774,7 +764,7 @@
       <c r="B11" s="3">
         <v>8</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="2"/>
@@ -786,8 +776,8 @@
       <c r="B12" s="3">
         <v>9</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>45</v>
+      <c r="C12" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -952,11 +942,11 @@
       <c r="D28" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="1" t="s">
@@ -1040,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
@@ -1055,7 +1045,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
@@ -1103,7 +1093,7 @@
         <v>17</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1118,7 +1108,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1129,8 +1119,8 @@
       <c r="B42" s="4">
         <v>10</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>46</v>
+      <c r="C42" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
@@ -1144,8 +1134,8 @@
       <c r="B43" s="3">
         <v>11</v>
       </c>
-      <c r="C43" s="14" t="s">
-        <v>47</v>
+      <c r="C43" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
@@ -1241,11 +1231,11 @@
       <c r="E51" s="2"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="19"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="16"/>
     </row>
     <row r="54" spans="1:5">
       <c r="B54" s="1" t="s">
@@ -1265,7 +1255,7 @@
       <c r="B55" s="3">
         <v>0</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C55" s="13" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="2"/>
@@ -1301,11 +1291,11 @@
       <c r="D58" s="2"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="19"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="16"/>
     </row>
     <row r="61" spans="1:5">
       <c r="B61" s="6" t="s">
@@ -1326,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D62" s="2"/>
     </row>
@@ -1338,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D63" s="2"/>
     </row>
@@ -1349,8 +1339,8 @@
       <c r="B64" s="3">
         <v>2</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>29</v>
+      <c r="C64" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="D64" s="2"/>
     </row>
@@ -1361,8 +1351,8 @@
       <c r="B65" s="3">
         <v>3</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>48</v>
+      <c r="C65" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="D65" s="2"/>
     </row>
@@ -1373,7 +1363,7 @@
       <c r="B66" s="5">
         <v>4</v>
       </c>
-      <c r="C66" s="9" t="s">
+      <c r="C66" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D66" s="2"/>
@@ -1385,7 +1375,7 @@
       <c r="B67" s="5">
         <v>5</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D67" s="2"/>
@@ -1397,7 +1387,7 @@
       <c r="B68" s="5">
         <v>6</v>
       </c>
-      <c r="C68" s="9" t="s">
+      <c r="C68" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D68" s="2"/>
@@ -1413,11 +1403,11 @@
       <c r="D69" s="2"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="19"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="1:4">
       <c r="B72" s="6" t="s">
@@ -1432,43 +1422,43 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="15" t="s">
-        <v>41</v>
+      <c r="C74" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="15" t="s">
-        <v>42</v>
+      <c r="C75" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B76" s="3">
         <v>3</v>
@@ -1480,7 +1470,7 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B77" s="5">
         <v>4</v>
@@ -1492,7 +1482,7 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B78" s="5">
         <v>5</v>
@@ -1504,7 +1494,7 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B79" s="5">
         <v>6</v>
@@ -1514,7 +1504,7 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B80" s="5">
         <v>7</v>
@@ -1531,6 +1521,7 @@
     <mergeCell ref="B71:D71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
AdjustHandPosition UP and DOWN coded.
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="21108" windowHeight="8688"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21915" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Channel Assignments" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -114,9 +115,6 @@
     <t>driveTrainEncoderR_B</t>
   </si>
   <si>
-    <t>buzzer</t>
-  </si>
-  <si>
     <t>driveTrainEncoderL_A</t>
   </si>
   <si>
@@ -163,13 +161,16 @@
   </si>
   <si>
     <t>liftEncoderB</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +195,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,6 +328,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -330,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -422,6 +432,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -456,6 +467,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -631,30 +643,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -665,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -673,11 +685,11 @@
         <v>0</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -685,21 +697,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -709,7 +723,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -717,11 +731,11 @@
         <v>4</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -729,11 +743,11 @@
         <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -745,7 +759,7 @@
       </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -757,7 +771,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -769,7 +783,7 @@
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -777,11 +791,11 @@
         <v>9</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -791,7 +805,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -801,7 +815,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>7</v>
       </c>
@@ -811,7 +825,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>7</v>
       </c>
@@ -821,7 +835,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -831,7 +845,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -841,7 +855,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
@@ -851,7 +865,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -861,7 +875,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
@@ -871,7 +885,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -881,7 +895,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -891,7 +905,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
@@ -901,7 +915,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
@@ -911,7 +925,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -921,7 +935,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
@@ -931,7 +945,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
@@ -941,14 +955,14 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="14" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
@@ -962,7 +976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -977,7 +991,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -992,7 +1006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1021,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1022,7 +1036,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1030,14 +1044,14 @@
         <v>4</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1045,14 +1059,14 @@
         <v>5</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>6</v>
       </c>
@@ -1067,7 +1081,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1082,7 +1096,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1112,7 +1126,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>7</v>
       </c>
@@ -1120,14 +1134,14 @@
         <v>10</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>7</v>
       </c>
@@ -1135,14 +1149,14 @@
         <v>11</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>7</v>
       </c>
@@ -1153,7 +1167,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>7</v>
       </c>
@@ -1164,7 +1178,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>7</v>
       </c>
@@ -1175,7 +1189,7 @@
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1200,7 @@
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>7</v>
       </c>
@@ -1197,7 +1211,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1222,7 @@
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>7</v>
       </c>
@@ -1219,7 +1233,7 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>7</v>
       </c>
@@ -1230,14 +1244,14 @@
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="53" spans="1:5">
-      <c r="B53" s="14" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="16"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="C53" s="16"/>
+      <c r="D53" s="17"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>1</v>
       </c>
@@ -1248,19 +1262,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="3">
         <v>0</v>
       </c>
-      <c r="C55" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="C55" s="18"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1282,7 @@
       <c r="C56" s="9"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>6</v>
       </c>
@@ -1280,7 +1292,7 @@
       <c r="C57" s="9"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
@@ -1290,14 +1302,14 @@
       <c r="C58" s="9"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="60" spans="1:5">
-      <c r="B60" s="14" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="16"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="C60" s="16"/>
+      <c r="D60" s="17"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>1</v>
       </c>
@@ -1308,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>6</v>
       </c>
@@ -1316,11 +1328,11 @@
         <v>0</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1328,11 +1340,11 @@
         <v>1</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>6</v>
       </c>
@@ -1340,11 +1352,11 @@
         <v>2</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
@@ -1356,7 +1368,7 @@
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>7</v>
       </c>
@@ -1368,7 +1380,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1392,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>7</v>
       </c>
@@ -1392,7 +1404,7 @@
       </c>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>7</v>
       </c>
@@ -1402,14 +1414,14 @@
       <c r="C69" s="10"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="71" spans="1:4">
-      <c r="B71" s="14" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="16"/>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="C71" s="16"/>
+      <c r="D71" s="17"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" s="6" t="s">
         <v>1</v>
       </c>
@@ -1420,45 +1432,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B73" s="3">
         <v>0</v>
       </c>
       <c r="C73" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="17" t="s">
-        <v>43</v>
+      <c r="C74" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="17" t="s">
-        <v>44</v>
+      <c r="C75" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B76" s="3">
         <v>3</v>
@@ -1468,9 +1480,9 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B77" s="5">
         <v>4</v>
@@ -1480,9 +1492,9 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B78" s="5">
         <v>5</v>
@@ -1492,9 +1504,9 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B79" s="5">
         <v>6</v>
@@ -1502,9 +1514,9 @@
       <c r="C79" s="10"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B80" s="5">
         <v>7</v>
@@ -1526,24 +1538,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add power distribution panel
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
   <si>
     <t>Function</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>liftEncoderB</t>
+  </si>
+  <si>
+    <t>PDP Channel</t>
   </si>
 </sst>
 </file>
@@ -321,6 +324,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -329,9 +335,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -645,14 +648,15 @@
     <col min="3" max="3" width="23.6640625" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" s="1" t="s">
@@ -696,7 +700,9 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
@@ -821,7 +827,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -831,7 +837,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -841,7 +847,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
@@ -851,7 +857,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -861,7 +867,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" s="8" t="s">
         <v>7</v>
       </c>
@@ -871,7 +877,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="8" t="s">
         <v>7</v>
       </c>
@@ -881,7 +887,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -891,7 +897,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="8" t="s">
         <v>7</v>
       </c>
@@ -901,7 +907,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:6">
       <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
@@ -911,7 +917,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -921,7 +927,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" s="8" t="s">
         <v>7</v>
       </c>
@@ -931,7 +937,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:6">
       <c r="A28" s="8" t="s">
         <v>7</v>
       </c>
@@ -941,14 +947,14 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="14" t="s">
+    <row r="30" spans="1:6">
+      <c r="B30" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="16"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
@@ -961,8 +967,11 @@
       <c r="E31" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
         <v>6</v>
       </c>
@@ -976,8 +985,11 @@
       <c r="E32" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
         <v>6</v>
       </c>
@@ -991,8 +1003,11 @@
       <c r="E33" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1006,8 +1021,11 @@
       <c r="E34" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
         <v>6</v>
       </c>
@@ -1021,8 +1039,11 @@
       <c r="E35" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
         <v>6</v>
       </c>
@@ -1036,8 +1057,11 @@
       <c r="E36" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
         <v>6</v>
       </c>
@@ -1051,8 +1075,11 @@
       <c r="E37" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>6</v>
       </c>
@@ -1066,8 +1093,11 @@
       <c r="E38" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1081,8 +1111,11 @@
       <c r="E39" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
         <v>6</v>
       </c>
@@ -1096,8 +1129,11 @@
       <c r="E40" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
         <v>6</v>
       </c>
@@ -1111,8 +1147,11 @@
       <c r="E41" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="8" t="s">
         <v>7</v>
       </c>
@@ -1126,8 +1165,11 @@
       <c r="E42" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
         <v>7</v>
       </c>
@@ -1141,8 +1183,11 @@
       <c r="E43" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="8" t="s">
         <v>7</v>
       </c>
@@ -1152,8 +1197,9 @@
       <c r="C44" s="10"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="8" t="s">
         <v>7</v>
       </c>
@@ -1163,8 +1209,9 @@
       <c r="C45" s="10"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="8" t="s">
         <v>7</v>
       </c>
@@ -1174,8 +1221,9 @@
       <c r="C46" s="10"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="8" t="s">
         <v>7</v>
       </c>
@@ -1185,8 +1233,9 @@
       <c r="C47" s="10"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="8" t="s">
         <v>7</v>
       </c>
@@ -1196,8 +1245,9 @@
       <c r="C48" s="10"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="8" t="s">
         <v>7</v>
       </c>
@@ -1207,8 +1257,9 @@
       <c r="C49" s="10"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
         <v>7</v>
       </c>
@@ -1218,8 +1269,9 @@
       <c r="C50" s="10"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="8" t="s">
         <v>7</v>
       </c>
@@ -1229,15 +1281,16 @@
       <c r="C51" s="10"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="B53" s="14" t="s">
+      <c r="F51" s="2"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="B53" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="16"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="C53" s="16"/>
+      <c r="D53" s="17"/>
+    </row>
+    <row r="54" spans="1:6">
       <c r="B54" s="1" t="s">
         <v>1</v>
       </c>
@@ -1248,19 +1301,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B55" s="3">
         <v>0</v>
       </c>
-      <c r="C55" s="13" t="s">
-        <v>32</v>
-      </c>
+      <c r="C55" s="12"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1321,7 @@
       <c r="C56" s="9"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
         <v>6</v>
       </c>
@@ -1280,7 +1331,7 @@
       <c r="C57" s="9"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
         <v>6</v>
       </c>
@@ -1290,14 +1341,14 @@
       <c r="C58" s="9"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="60" spans="1:5">
-      <c r="B60" s="14" t="s">
+    <row r="60" spans="1:6">
+      <c r="B60" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="16"/>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="C60" s="16"/>
+      <c r="D60" s="17"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="B61" s="6" t="s">
         <v>1</v>
       </c>
@@ -1308,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
         <v>6</v>
       </c>
@@ -1320,7 +1371,7 @@
       </c>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1332,7 +1383,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
         <v>6</v>
       </c>
@@ -1403,11 +1454,11 @@
       <c r="D69" s="2"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C71" s="15"/>
-      <c r="D71" s="16"/>
+      <c r="C71" s="16"/>
+      <c r="D71" s="17"/>
     </row>
     <row r="72" spans="1:4">
       <c r="B72" s="6" t="s">
@@ -1439,7 +1490,7 @@
       <c r="B74" s="3">
         <v>1</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C74" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D74" s="2"/>
@@ -1451,7 +1502,7 @@
       <c r="B75" s="3">
         <v>2</v>
       </c>
-      <c r="C75" s="17" t="s">
+      <c r="C75" s="14" t="s">
         <v>44</v>
       </c>
       <c r="D75" s="2"/>

</xml_diff>

<commit_message>
Show digital channels that can't be used on MXP because they conflict with PWM.
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
   <si>
     <t>Function</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>PDP Channel</t>
+  </si>
+  <si>
+    <t>N/A (used by PWM)</t>
   </si>
 </sst>
 </file>
@@ -644,10 +647,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:F51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -803,7 +809,9 @@
       <c r="B13" s="3">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4">
@@ -813,7 +821,9 @@
       <c r="B14" s="5">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4">
@@ -1581,7 +1591,7 @@
     <mergeCell ref="B71:D71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup scale="93" fitToHeight="2" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fix shift direction and driving distance
</commit_message>
<xml_diff>
--- a/Robot Channels.xlsx
+++ b/Robot Channels.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="56">
   <si>
     <t>Function</t>
   </si>
@@ -139,12 +139,6 @@
   </si>
   <si>
     <t>liftRight</t>
-  </si>
-  <si>
-    <t>liftEncoderA</t>
-  </si>
-  <si>
-    <t>liftEncoderB</t>
   </si>
   <si>
     <t>Buzzer</t>
@@ -673,8 +667,8 @@
   </sheetPr>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -712,9 +706,7 @@
       <c r="B3" s="3">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="C3" s="12"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
@@ -724,9 +716,7 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="C4" s="12"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
@@ -737,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -831,7 +821,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2"/>
     </row>
@@ -843,7 +833,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -1008,7 +998,7 @@
         <v>13</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1455,7 +1445,7 @@
         <v>4</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D66" s="2"/>
     </row>
@@ -1521,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D73" s="2"/>
     </row>
@@ -1533,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D74" s="2"/>
     </row>
@@ -1545,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D75" s="2"/>
     </row>
@@ -1557,7 +1547,7 @@
         <v>3</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D76" s="2"/>
     </row>
@@ -1569,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D77" s="2"/>
     </row>
@@ -1581,7 +1571,7 @@
         <v>5</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D78" s="2"/>
     </row>
@@ -1611,55 +1601,55 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B81" s="3">
         <v>0</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B82" s="3">
         <v>1</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B83" s="3">
         <v>2</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B84" s="3">
         <v>3</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B85" s="5">
         <v>4</v>
@@ -1669,7 +1659,7 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B86" s="5">
         <v>5</v>
@@ -1679,7 +1669,7 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B87" s="5">
         <v>6</v>
@@ -1689,7 +1679,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B88" s="5">
         <v>7</v>

</xml_diff>